<commit_message>
Added import  lease sql file
</commit_message>
<xml_diff>
--- a/99-Shared/01-BSVoertuigEnKlantbeheer/Leasemaatschappijen voor de sitebouwers.xlsx
+++ b/99-Shared/01-BSVoertuigEnKlantbeheer/Leasemaatschappijen voor de sitebouwers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\EsraH\Caespi\99-Shared\01-BSVoertuigEnKlantbeheer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CasparE\Documents\Minor-GarageManagementSysteem\99-Shared\01-BSVoertuigEnKlantbeheer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -315,7 +315,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +330,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -352,9 +358,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,396 +647,903 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <f>"update Klant set  Telefoonnummer= '"&amp;B2&amp;"' WHERE ID="&amp;C2&amp;";"</f>
+        <v>update Klant set  Telefoonnummer= '040-7524753' WHERE ID=1;</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A2&amp;"' WHERE ID="&amp;C2&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= '123Carlease BV' WHERE ID=1;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f t="shared" ref="D3:D47" si="0">"update Klant set  Telefoonnummer= '"&amp;B3&amp;"' WHERE ID="&amp;C3&amp;";"</f>
+        <v>update Klant set  Telefoonnummer= '020-5622402' WHERE ID=2;</v>
+      </c>
+      <c r="E3" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A3&amp;"' WHERE ID="&amp;C3&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= '@ AutoLeaseCenter B.V.' WHERE ID=2;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '040-7824776' WHERE ID=3;</v>
+      </c>
+      <c r="E4" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A4&amp;"' WHERE ID="&amp;C4&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'ActivLease' WHERE ID=3;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '010-3622327' WHERE ID=4;</v>
+      </c>
+      <c r="E5" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A5&amp;"' WHERE ID="&amp;C5&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'ALD Automotive' WHERE ID=4;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '016-1023251' WHERE ID=5;</v>
+      </c>
+      <c r="E6" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A6&amp;"' WHERE ID="&amp;C6&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Arval' WHERE ID=5;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '030-4015128' WHERE ID=6;</v>
+      </c>
+      <c r="E7" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A7&amp;"' WHERE ID="&amp;C7&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Autobedrijf Arjan van Houtum' WHERE ID=6;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '037-021816' WHERE ID=7;</v>
+      </c>
+      <c r="E8" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A8&amp;"' WHERE ID="&amp;C8&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Autolease Twente B.V.' WHERE ID=7;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>92</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '049-435590' WHERE ID=8;</v>
+      </c>
+      <c r="E9" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A9&amp;"' WHERE ID="&amp;C9&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Autoradam Almere Oost B.V.' WHERE ID=8;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '040-3125114' WHERE ID=9;</v>
+      </c>
+      <c r="E10" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A10&amp;"' WHERE ID="&amp;C10&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'B.V. Multirent' WHERE ID=9;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '020-4720786' WHERE ID=10;</v>
+      </c>
+      <c r="E11" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A11&amp;"' WHERE ID="&amp;C11&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Blankert Shortlease BV' WHERE ID=10;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '040-5513479' WHERE ID=11;</v>
+      </c>
+      <c r="E12" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A12&amp;"' WHERE ID="&amp;C12&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Boxsons Lease' WHERE ID=11;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '040-6119338' WHERE ID=12;</v>
+      </c>
+      <c r="E13" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A13&amp;"' WHERE ID="&amp;C13&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Bronkhorst Lease B.V.' WHERE ID=12;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '020-897465' WHERE ID=13;</v>
+      </c>
+      <c r="E14" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A14&amp;"' WHERE ID="&amp;C14&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Daimler Fleet Management' WHERE ID=13;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '010-0313928' WHERE ID=14;</v>
+      </c>
+      <c r="E15" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A15&amp;"' WHERE ID="&amp;C15&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Financial Lease Apeldoorn' WHERE ID=14;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '040-8624695' WHERE ID=15;</v>
+      </c>
+      <c r="E16" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A16&amp;"' WHERE ID="&amp;C16&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Financiele Lease Nederland BV' WHERE ID=15;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '040-395804' WHERE ID=16;</v>
+      </c>
+      <c r="E17" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A17&amp;"' WHERE ID="&amp;C17&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Fred Janssen Autogroep' WHERE ID=16;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '030-58870' WHERE ID=17;</v>
+      </c>
+      <c r="E18" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A18&amp;"' WHERE ID="&amp;C18&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'H4 Car Lease' WHERE ID=17;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '042-2519823' WHERE ID=18;</v>
+      </c>
+      <c r="E19" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A19&amp;"' WHERE ID="&amp;C19&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Interlease &amp; Rent BV' WHERE ID=18;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '040-6418749' WHERE ID=19;</v>
+      </c>
+      <c r="E20" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A20&amp;"' WHERE ID="&amp;C20&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'KeyCar B.V.' WHERE ID=19;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '047-4012366' WHERE ID=20;</v>
+      </c>
+      <c r="E21" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A21&amp;"' WHERE ID="&amp;C21&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Koolen Auto's BV' WHERE ID=20;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '030-5212427' WHERE ID=21;</v>
+      </c>
+      <c r="E22" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A22&amp;"' WHERE ID="&amp;C22&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Lease2Move B.V.' WHERE ID=21;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
       <c r="B23" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '040-9124884' WHERE ID=22;</v>
+      </c>
+      <c r="E23" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A23&amp;"' WHERE ID="&amp;C23&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'LeaseBijtellingVrij.nl' WHERE ID=22;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '038-0114481' WHERE ID=23;</v>
+      </c>
+      <c r="E24" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A24&amp;"' WHERE ID="&amp;C24&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'LeaseLinq' WHERE ID=23;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
       <c r="B25" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '030-9423214' WHERE ID=24;</v>
+      </c>
+      <c r="E25" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A25&amp;"' WHERE ID="&amp;C25&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'LeaseOnline' WHERE ID=24;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
       <c r="B26" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '030-3216771' WHERE ID=25;</v>
+      </c>
+      <c r="E26" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A26&amp;"' WHERE ID="&amp;C26&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'LeaseParcours.nl' WHERE ID=25;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
       <c r="B27" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '016-2812210' WHERE ID=26;</v>
+      </c>
+      <c r="E27" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A27&amp;"' WHERE ID="&amp;C27&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'LeasePlan Nederland N.V.' WHERE ID=26;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>51</v>
       </c>
       <c r="B28" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '047-1725195' WHERE ID=27;</v>
+      </c>
+      <c r="E28" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A28&amp;"' WHERE ID="&amp;C28&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'LeaseRoute B.V.' WHERE ID=27;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
       <c r="B29" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '040-0724829' WHERE ID=28;</v>
+      </c>
+      <c r="E29" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A29&amp;"' WHERE ID="&amp;C29&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Leasevrij.nl' WHERE ID=28;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
       <c r="B30" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>29</v>
+      </c>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '010-3623743' WHERE ID=29;</v>
+      </c>
+      <c r="E30" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A30&amp;"' WHERE ID="&amp;C30&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Lexus Enschede' WHERE ID=29;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>57</v>
       </c>
       <c r="B31" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '048-314291' WHERE ID=30;</v>
+      </c>
+      <c r="E31" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A31&amp;"' WHERE ID="&amp;C31&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Middelbeek Lease' WHERE ID=30;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>59</v>
       </c>
       <c r="B32" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>31</v>
+      </c>
+      <c r="D32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '010-3023485' WHERE ID=31;</v>
+      </c>
+      <c r="E32" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A32&amp;"' WHERE ID="&amp;C32&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Omni Lease B.V.' WHERE ID=31;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>61</v>
       </c>
       <c r="B33" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>32</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '010-9514761' WHERE ID=32;</v>
+      </c>
+      <c r="E33" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A33&amp;"' WHERE ID="&amp;C33&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'OnlineAutoLeasen.nl  |  DBL Lease &amp; Finance' WHERE ID=32;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>63</v>
       </c>
       <c r="B34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>33</v>
+      </c>
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '020-7711730' WHERE ID=33;</v>
+      </c>
+      <c r="E34" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A34&amp;"' WHERE ID="&amp;C34&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Oxonia Lease' WHERE ID=33;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>65</v>
       </c>
       <c r="B35" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>34</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '047-834087' WHERE ID=34;</v>
+      </c>
+      <c r="E35" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A35&amp;"' WHERE ID="&amp;C35&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Releasecompany' WHERE ID=34;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>67</v>
       </c>
       <c r="B36" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>35</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '010-5623223' WHERE ID=35;</v>
+      </c>
+      <c r="E36" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A36&amp;"' WHERE ID="&amp;C36&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Shortlease Auto Nederland' WHERE ID=35;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>69</v>
       </c>
       <c r="B37" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>36</v>
+      </c>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '033-1012894' WHERE ID=36;</v>
+      </c>
+      <c r="E37" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A37&amp;"' WHERE ID="&amp;C37&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Supershortlease.nl' WHERE ID=36;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>71</v>
       </c>
       <c r="B38" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>37</v>
+      </c>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '030-68659' WHERE ID=37;</v>
+      </c>
+      <c r="E38" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A38&amp;"' WHERE ID="&amp;C38&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Terberg Leasing B.V.' WHERE ID=37;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>73</v>
       </c>
       <c r="B39" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>38</v>
+      </c>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '040-4820473' WHERE ID=38;</v>
+      </c>
+      <c r="E39" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A39&amp;"' WHERE ID="&amp;C39&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'That's Lease' WHERE ID=38;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>75</v>
       </c>
       <c r="B40" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>39</v>
+      </c>
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '010-5824114' WHERE ID=39;</v>
+      </c>
+      <c r="E40" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A40&amp;"' WHERE ID="&amp;C40&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'TopSportLease' WHERE ID=39;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>77</v>
       </c>
       <c r="B41" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>40</v>
+      </c>
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '040-2121275' WHERE ID=40;</v>
+      </c>
+      <c r="E41" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A41&amp;"' WHERE ID="&amp;C41&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Total Car Lease B.V.' WHERE ID=40;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>79</v>
       </c>
       <c r="B42" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>41</v>
+      </c>
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '020-2915476' WHERE ID=41;</v>
+      </c>
+      <c r="E42" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A42&amp;"' WHERE ID="&amp;C42&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Vallei Autolease B.V.' WHERE ID=41;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>81</v>
       </c>
       <c r="B43" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>42</v>
+      </c>
+      <c r="D43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '010-6713542' WHERE ID=42;</v>
+      </c>
+      <c r="E43" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A43&amp;"' WHERE ID="&amp;C43&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Van Renselaar Cars' WHERE ID=42;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>83</v>
       </c>
       <c r="B44" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>43</v>
+      </c>
+      <c r="D44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '028-8422529' WHERE ID=43;</v>
+      </c>
+      <c r="E44" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A44&amp;"' WHERE ID="&amp;C44&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Vemo Lease BV' WHERE ID=43;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>85</v>
       </c>
       <c r="B45" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>44</v>
+      </c>
+      <c r="D45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '030-995346' WHERE ID=44;</v>
+      </c>
+      <c r="E45" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A45&amp;"' WHERE ID="&amp;C45&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Verkerk Lease' WHERE ID=44;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>87</v>
       </c>
       <c r="B46" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>45</v>
+      </c>
+      <c r="D46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '011-947473' WHERE ID=45;</v>
+      </c>
+      <c r="E46" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A46&amp;"' WHERE ID="&amp;C46&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Voorraadlease Kiezen &amp; Rijden' WHERE ID=45;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>89</v>
       </c>
       <c r="B47" t="s">
         <v>90</v>
       </c>
+      <c r="C47">
+        <v>46</v>
+      </c>
+      <c r="D47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>update Klant set  Telefoonnummer= '010-305750' WHERE ID=46;</v>
+      </c>
+      <c r="E47" t="str">
+        <f>"update Leasemaatschappij set  Naam= '"&amp;A47&amp;"' WHERE ID="&amp;C47&amp;";"</f>
+        <v>update Leasemaatschappij set  Naam= 'Zuidlease B.V.' WHERE ID=46;</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B47"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>